<commit_message>
spreadsheet: support sorting a sheet
The file format doesn't support sorting, so we
need to sort the sheet rows and renumber after sorting.
</commit_message>
<xml_diff>
--- a/_examples/spreadsheet/sort-filter/sort-filter.xlsx
+++ b/_examples/spreadsheet/sort-filter/sort-filter.xlsx
@@ -93,24 +93,24 @@
     </ma:row>
     <ma:row r="2">
       <ma:c r="A2" t="s">
-        <ma:v>3</ma:v>
+        <ma:v>7</ma:v>
       </ma:c>
       <ma:c r="B2" t="n">
-        <ma:v>2</ma:v>
+        <ma:v>6</ma:v>
       </ma:c>
       <ma:c r="C2" t="n">
-        <ma:v>1</ma:v>
+        <ma:v>13</ma:v>
       </ma:c>
     </ma:row>
     <ma:row r="3">
       <ma:c r="A3" t="s">
-        <ma:v>4</ma:v>
+        <ma:v>6</ma:v>
       </ma:c>
       <ma:c r="B3" t="n">
-        <ma:v>3</ma:v>
+        <ma:v>5</ma:v>
       </ma:c>
       <ma:c r="C3" t="n">
-        <ma:v>4</ma:v>
+        <ma:v>10</ma:v>
       </ma:c>
     </ma:row>
     <ma:row r="4">
@@ -126,24 +126,24 @@
     </ma:row>
     <ma:row r="5">
       <ma:c r="A5" t="s">
-        <ma:v>6</ma:v>
+        <ma:v>4</ma:v>
       </ma:c>
       <ma:c r="B5" t="n">
-        <ma:v>5</ma:v>
+        <ma:v>3</ma:v>
       </ma:c>
       <ma:c r="C5" t="n">
-        <ma:v>10</ma:v>
+        <ma:v>4</ma:v>
       </ma:c>
     </ma:row>
     <ma:row r="6">
       <ma:c r="A6" t="s">
-        <ma:v>7</ma:v>
+        <ma:v>3</ma:v>
       </ma:c>
       <ma:c r="B6" t="n">
-        <ma:v>6</ma:v>
+        <ma:v>2</ma:v>
       </ma:c>
       <ma:c r="C6" t="n">
-        <ma:v>13</ma:v>
+        <ma:v>1</ma:v>
       </ma:c>
     </ma:row>
   </ma:sheetData>

</xml_diff>